<commit_message>
Woche 9 (KW51: 16.12. - 22.12.2024)
</commit_message>
<xml_diff>
--- a/Kosten.xlsx
+++ b/Kosten.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nbg6156.sharepoint.com/sites/EAV2426s_IT-Speedster/Shared Documents/Speedster/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="116" documentId="8_{ACC801FD-4E1C-41DC-A0BB-42FD5953A661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5FB0180-9D8A-40C0-826D-7262D9563B94}"/>
+  <xr:revisionPtr revIDLastSave="128" documentId="8_{ACC801FD-4E1C-41DC-A0BB-42FD5953A661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9B3F194-227A-4A97-B307-7CA3C12917C3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{10CE70E1-3845-4303-83F7-C1745ACA87B9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{10CE70E1-3845-4303-83F7-C1745ACA87B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>Kostenträger</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Akku Lipo 2200mAh mit Ladegerät</t>
   </si>
   <si>
-    <t>Deans-T-Adapter</t>
-  </si>
-  <si>
     <t>Motor (mit ESC)</t>
   </si>
   <si>
@@ -105,6 +102,15 @@
   </si>
   <si>
     <t>Bezeichnung</t>
+  </si>
+  <si>
+    <t>3D-Druck Filament pauschal</t>
+  </si>
+  <si>
+    <t>sonstige Verbrauchsmaterialien pauschal</t>
+  </si>
+  <si>
+    <t>alle</t>
   </si>
 </sst>
 </file>
@@ -638,32 +644,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51B529B-B5E4-484E-A6BF-E38448F6C170}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" style="15" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.77734375" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="11.44140625" style="2"/>
+    <col min="1" max="1" width="40.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>9</v>
@@ -675,7 +681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -696,7 +702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -710,14 +716,14 @@
         <v>1</v>
       </c>
       <c r="E3" s="6">
-        <f t="shared" ref="E3:E19" si="0">IF(B3&gt;0,(C3/B3)*D3,"")</f>
+        <f t="shared" ref="E3:E18" si="0">IF(B3&gt;0,(C3/B3)*D3,"")</f>
         <v>25.39</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -738,7 +744,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -759,7 +765,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -780,7 +786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -801,7 +807,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -822,7 +828,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
@@ -843,7 +849,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
@@ -864,70 +870,70 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C11" s="5">
-        <v>7.99</v>
+        <v>31.28</v>
       </c>
       <c r="D11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>31.28</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C12" s="5">
-        <v>31.28</v>
+        <v>8.09</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
       </c>
       <c r="E12" s="6">
         <f t="shared" si="0"/>
-        <v>31.28</v>
+        <v>2.0225</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C13" s="5">
-        <v>8.09</v>
+        <v>11.44</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
       </c>
       <c r="E13" s="6">
         <f t="shared" si="0"/>
-        <v>2.0225</v>
+        <v>2.2879999999999998</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>18</v>
       </c>
@@ -935,52 +941,62 @@
         <v>5</v>
       </c>
       <c r="C14" s="5">
-        <v>11.44</v>
+        <v>22.36</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
       </c>
       <c r="E14" s="6">
         <f t="shared" si="0"/>
-        <v>2.2879999999999998</v>
+        <v>4.4719999999999995</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B15" s="4">
+        <v>1</v>
+      </c>
+      <c r="C15" s="5">
+        <v>20</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
+      <c r="E15" s="6">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="4">
+        <v>1</v>
+      </c>
+      <c r="C16" s="5">
         <v>5</v>
       </c>
-      <c r="C15" s="5">
-        <v>22.36</v>
-      </c>
-      <c r="D15" s="4">
-        <v>1</v>
-      </c>
-      <c r="E15" s="6">
-        <f t="shared" si="0"/>
-        <v>4.4719999999999995</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
+      <c r="E16" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
@@ -991,43 +1007,32 @@
       </c>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="4"/>
+    <row r="18" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="8"/>
       <c r="E18" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F19" s="7"/>
-    </row>
-    <row r="20" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="10" t="s">
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="12">
-        <f>SUM(C2:C19)</f>
-        <v>246.17000000000002</v>
-      </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="13">
-        <f>SUM(E2:E19)</f>
-        <v>167.36083333333335</v>
-      </c>
-      <c r="F20" s="14"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="12">
+        <f>SUM(C2:C18)</f>
+        <v>263.18</v>
+      </c>
+      <c r="D19" s="16"/>
+      <c r="E19" s="13">
+        <f>SUM(E2:E18)</f>
+        <v>192.36083333333335</v>
+      </c>
+      <c r="F19" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1045,6 +1050,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005D41303A6B244740A2799A34F49334A8" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dee341bca2430f0ef2b01f5606762eda">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e0d6cc59-ea8b-4001-8093-37243f0a69e3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f039fa3c113edae47fee5e02d564d92" ns2:_="">
     <xsd:import namespace="e0d6cc59-ea8b-4001-8093-37243f0a69e3"/>
@@ -1228,15 +1242,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6AC114D5-950D-4A04-9A10-93041372E37F}">
   <ds:schemaRefs>
@@ -1254,6 +1259,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D37260D8-6E66-42DE-AB41-BF29A5DDA730}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB3BEC89-47B9-4621-B23B-75071F83DCDE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1269,12 +1282,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D37260D8-6E66-42DE-AB41-BF29A5DDA730}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>